<commit_message>
changed generate list from static code to a function, plan to change it further to allow the list to update when an item is added
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,6 +531,50 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Cat</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>incomplete</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2025-01-05 21:33:59.848542</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>at</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>incomplete</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2025-01-05 21:38:36.142019</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added a function to clear old tasks and can now delete tasks with other function del_task
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,138 +443,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Clean Dishes</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>incomplete</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2025-01-04 20:32:35.766134</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>play with cats</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>incomplete</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2025-01-04 20:39:39.801492</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>play with cats</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>incomplete</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2025-01-04 20:41:58.354746</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>add</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>incomplete</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2025-01-04 20:44:13.878524</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Cat</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>incomplete</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2025-01-05 21:33:59.848542</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>at</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>incomplete</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>2025-01-05 21:38:36.142019</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Have reattached the functions, but having issues with sizing and scrolling correctly after adding / deleting tasks from the todoList and generating them on the canvas
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,6 +443,50 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>incomplete</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2025-01-10 15:57:00.352011</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>incomplete</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2025-01-10 15:57:00.499081</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>